<commit_message>
browser platform dynamic complete
</commit_message>
<xml_diff>
--- a/examples/DropsTestRunDefinition.xlsx
+++ b/examples/DropsTestRunDefinition.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24555" windowHeight="11670" activeTab="3"/>
+    <workbookView windowWidth="28800" windowHeight="12540" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TestRun" sheetId="1" r:id="rId1"/>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
   <si>
     <t>Attribute</t>
   </si>
@@ -174,6 +174,15 @@
   </si>
   <si>
     <t>Mobile</t>
+  </si>
+  <si>
+    <t>platformName</t>
+  </si>
+  <si>
+    <t>deviceName</t>
+  </si>
+  <si>
+    <t>platfomrVersion</t>
   </si>
   <si>
     <t>GC.CLASSES_TESTCASE</t>
@@ -256,9 +265,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
@@ -292,7 +301,135 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -301,134 +438,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -456,13 +465,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -474,169 +633,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -652,10 +661,17 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -672,6 +688,32 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -714,182 +756,149 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1396,13 +1405,13 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="1" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="23.8333333333333" customWidth="1"/>
     <col min="2" max="2" width="15.5" customWidth="1"/>
@@ -1410,9 +1419,12 @@
     <col min="4" max="4" width="16.25" customWidth="1"/>
     <col min="5" max="5" width="20.25" customWidth="1"/>
     <col min="6" max="6" width="19.125" customWidth="1"/>
+    <col min="8" max="8" width="22.375" customWidth="1"/>
+    <col min="9" max="9" width="20.25" customWidth="1"/>
+    <col min="10" max="10" width="23.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -1434,6 +1446,15 @@
       <c r="G1" t="s">
         <v>28</v>
       </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
@@ -1443,13 +1464,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>26</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1483,13 +1504,13 @@
         <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1503,7 +1524,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1529,6 +1550,7 @@
     <col min="4" max="4" width="23.6666666666667" customWidth="1"/>
     <col min="5" max="5" width="16.5" customWidth="1"/>
     <col min="7" max="7" width="54.3333333333333" customWidth="1"/>
+    <col min="8" max="8" width="35.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -1539,37 +1561,37 @@
         <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" t="s">
         <v>36</v>
-      </c>
-      <c r="F1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J1" t="s">
-        <v>40</v>
-      </c>
-      <c r="K1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L1" t="s">
-        <v>42</v>
-      </c>
-      <c r="M1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1586,10 +1608,10 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1606,16 +1628,16 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="K3">
         <v>5</v>
@@ -1635,19 +1657,19 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="K4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1664,13 +1686,13 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="G5" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>